<commit_message>
fixed bugs and test case working
fixed out of bounds bug for name array with if/else statement, commented out unecessary tests
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -139,12 +139,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Quartet Mozart</t>
-  </si>
-  <si>
-    <t>Johnny Bravo</t>
-  </si>
-  <si>
     <t>ED</t>
   </si>
   <si>
@@ -184,7 +178,13 @@
     <t>322-3486</t>
   </si>
   <si>
-    <t>James John (New)</t>
+    <t>James Johns (New)</t>
+  </si>
+  <si>
+    <t>Quartet Mozarts</t>
+  </si>
+  <si>
+    <t>Johnny Bravos</t>
   </si>
 </sst>
 </file>
@@ -918,7 +918,7 @@
   <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1108,13 +1108,13 @@
         <v>26</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" s="40">
         <v>3661</v>
@@ -1145,16 +1145,16 @@
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="40" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E10" s="36" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G10" s="40">
         <v>4521</v>
@@ -1166,16 +1166,16 @@
         <v>5621</v>
       </c>
       <c r="J10" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="42" t="s">
         <v>35</v>
-      </c>
-      <c r="K10" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="42" t="s">
-        <v>37</v>
       </c>
       <c r="O10" s="6"/>
     </row>
@@ -1185,16 +1185,16 @@
       </c>
       <c r="B11" s="35"/>
       <c r="C11" s="40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11" s="36">
         <v>2315</v>
@@ -1206,16 +1206,16 @@
         <v>5324</v>
       </c>
       <c r="J11" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="37" t="s">
         <v>39</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="37" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>